<commit_message>
Update NWNDS Desert Master List.xlsx
</commit_message>
<xml_diff>
--- a/_notes_/Encounter Tables/NWNDS Desert Master List.xlsx
+++ b/_notes_/Encounter Tables/NWNDS Desert Master List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5131" uniqueCount="1481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5135" uniqueCount="1482">
   <si>
     <t>Name</t>
   </si>
@@ -4463,6 +4463,9 @@
   </si>
   <si>
     <t>Beetle, Shaqat: 01 HD</t>
+  </si>
+  <si>
+    <t>1 to 24</t>
   </si>
 </sst>
 </file>
@@ -4607,7 +4610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4669,6 +4672,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4893,10 +4899,10 @@
   <dimension ref="A1:AA1028"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B209" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B145" sqref="A145:B145"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1"/>
@@ -10538,7 +10544,9 @@
       <c r="J121" s="15">
         <v>5</v>
       </c>
-      <c r="K121" s="15"/>
+      <c r="K121" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="L121" s="15" t="s">
         <v>101</v>
       </c>
@@ -10595,7 +10603,9 @@
       <c r="L122" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="M122" s="15"/>
+      <c r="M122" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="N122" s="15"/>
       <c r="O122" s="15"/>
       <c r="P122" s="15"/>
@@ -12860,8 +12870,8 @@
       <c r="K171" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="L171" s="15">
-        <v>1</v>
+      <c r="L171" s="21" t="s">
+        <v>48</v>
       </c>
       <c r="M171" s="15" t="s">
         <v>33</v>
@@ -13260,7 +13270,7 @@
       <c r="O180" s="15"/>
       <c r="P180" s="15"/>
     </row>
-    <row r="181" spans="1:27" ht="25.5">
+    <row r="181" spans="1:27">
       <c r="A181" s="15" t="s">
         <v>1109</v>
       </c>
@@ -13268,7 +13278,7 @@
         <v>91</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D181" s="15" t="s">
         <v>18</v>
@@ -13293,7 +13303,7 @@
         <v>89</v>
       </c>
       <c r="L181" s="15" t="s">
-        <v>1474</v>
+        <v>1481</v>
       </c>
       <c r="M181" s="15" t="s">
         <v>26</v>
@@ -13332,8 +13342,8 @@
       <c r="F182" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G182" s="19">
-        <v>4</v>
+      <c r="G182" s="19" t="s">
+        <v>948</v>
       </c>
       <c r="H182" s="15">
         <v>5</v>

</xml_diff>